<commit_message>
Add large values after 2 seeds
</commit_message>
<xml_diff>
--- a/baseline.xlsx
+++ b/baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meine Ablage\Masterarbeit\fantastic-umbrella\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221C321E-8125-4223-B93D-68DCA7D673C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86435ED-8D53-4BA4-9C2B-582D661E93FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{4DBCF66B-BE6D-4CD2-ACFF-1BE78E9C1634}"/>
+    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="15400" xr2:uid="{4DBCF66B-BE6D-4CD2-ACFF-1BE78E9C1634}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
   <si>
     <t>Task</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Metric</t>
   </si>
   <si>
-    <t>Training time</t>
-  </si>
-  <si>
     <t>CoLA</t>
   </si>
   <si>
@@ -113,15 +110,6 @@
     <t>65.70</t>
   </si>
   <si>
-    <t>Result (GitHub, Validation, Base)</t>
-  </si>
-  <si>
-    <t>BERT_base Paper</t>
-  </si>
-  <si>
-    <t>BERT_large Paper</t>
-  </si>
-  <si>
     <t>52.1</t>
   </si>
   <si>
@@ -246,6 +234,69 @@
   </si>
   <si>
     <t>0.29/0.2</t>
+  </si>
+  <si>
+    <t>BERT BASE</t>
+  </si>
+  <si>
+    <t>Result (GitHub, Validation)</t>
+  </si>
+  <si>
+    <t>Paper</t>
+  </si>
+  <si>
+    <t>BERT LARGE</t>
+  </si>
+  <si>
+    <t>59.94</t>
+  </si>
+  <si>
+    <t>0.54</t>
+  </si>
+  <si>
+    <t>61.08</t>
+  </si>
+  <si>
+    <t>0.52</t>
+  </si>
+  <si>
+    <t>93.58</t>
+  </si>
+  <si>
+    <t>0.08</t>
+  </si>
+  <si>
+    <t>93.92</t>
+  </si>
+  <si>
+    <t>0.32</t>
+  </si>
+  <si>
+    <t>91.28/87.5</t>
+  </si>
+  <si>
+    <t>6.23/9.36</t>
+  </si>
+  <si>
+    <t>91/87.96</t>
+  </si>
+  <si>
+    <t>0.06/0.01</t>
+  </si>
+  <si>
+    <t>86.35/886.2</t>
+  </si>
+  <si>
+    <t>0.03/0.24</t>
+  </si>
+  <si>
+    <t>91.85</t>
+  </si>
+  <si>
+    <t>75.09</t>
+  </si>
+  <si>
+    <t>0.434</t>
   </si>
 </sst>
 </file>
@@ -289,21 +340,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -316,6 +358,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -630,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA4993B-FA11-4D77-8FDF-E0D7655297E0}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:I7"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -642,29 +687,29 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>23</v>
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
@@ -672,252 +717,353 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="H4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="F5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="G5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="H5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="I5" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="I9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" s="6" t="s">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="D11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="E11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="F11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="G11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="H11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="I11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="6" t="s">
+    </row>
+    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="B13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="3">
-        <v>0.13680555555555554</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1.0875000000000001</v>
-      </c>
-      <c r="D10" s="3">
-        <v>9.7916666666666666E-2</v>
-      </c>
-      <c r="E10" s="3">
-        <v>9.2361111111111116E-2</v>
-      </c>
-      <c r="F10" s="5">
-        <v>9.8912037037037034E-2</v>
-      </c>
-      <c r="G10" s="5">
-        <v>0.10790509259259258</v>
-      </c>
-      <c r="H10" s="4">
-        <v>1.70625</v>
-      </c>
-      <c r="I10" s="2">
-        <v>57</v>
+      <c r="B15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>